<commit_message>
experiments set up final
</commit_message>
<xml_diff>
--- a/Human experiment 2.xlsx
+++ b/Human experiment 2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryamad/Google Drive/2022/Dissertation/conditional_diffusion_simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9286C872-FEFE-4B42-9365-6B9392515B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B92ABEA-ECA2-B44E-A833-907B5D85E0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{42B1DF19-554C-3E44-9726-32D98B11BA69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,25 +36,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>METHOD</t>
   </si>
   <si>
     <t>DOES IT LOOK LIKE A NUMBER? (1/0)</t>
   </si>
+  <si>
+    <t>CDE</t>
+  </si>
+  <si>
+    <t>CDIFFE</t>
+  </si>
+  <si>
+    <t>SMC</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,8 +98,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4FD5B5-88DA-E543-B358-8FAF255CB3C0}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:I201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -405,11 +427,1072 @@
     <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>SUMIF(A2:A201, 0, B2:B201)</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>H2/50 * 100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f>SUMIF(A2:A201, 1, B2:B201)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I5" si="0">H3/50 * 100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f>SUMIF(A2:A201, 2, B2:B201)</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f>SUMIF(A2:A201, 3, B2:B201)</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201">
         <v>1</v>
       </c>
     </row>

</xml_diff>